<commit_message>
update colors, add to analysis
</commit_message>
<xml_diff>
--- a/data/DCR-Deaths-in-Custody-Jan-2020-to-March-2025.xlsx
+++ b/data/DCR-Deaths-in-Custody-Jan-2020-to-March-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\wv_deaths_in_custody\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37619CF6-0B31-42D2-A0C1-209AA7BBBBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170FB68-A943-4FDB-B2C7-DCE7F55F770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26925" yWindow="3600" windowWidth="21600" windowHeight="11235" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="867">
   <si>
     <t>1/15/2020</t>
   </si>
@@ -1970,9 +1970,6 @@
   </si>
   <si>
     <t>23-F-345</t>
-  </si>
-  <si>
-    <t>|PTF Pretrial Felon</t>
   </si>
   <si>
     <t>4/30/2024</t>
@@ -2636,12 +2633,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2718,24 +2722,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -3244,7 +3249,7 @@
         <v>8</v>
       </c>
       <c r="J6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3340,7 +3345,7 @@
         <v>40</v>
       </c>
       <c r="J9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3436,7 +3441,7 @@
         <v>8</v>
       </c>
       <c r="J12" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3468,7 +3473,7 @@
         <v>54</v>
       </c>
       <c r="J13" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3532,7 +3537,7 @@
         <v>61</v>
       </c>
       <c r="J15" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3628,7 +3633,7 @@
         <v>40</v>
       </c>
       <c r="J18" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3660,7 +3665,7 @@
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3692,7 +3697,7 @@
         <v>40</v>
       </c>
       <c r="J20" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3788,7 +3793,7 @@
         <v>8</v>
       </c>
       <c r="J23" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3884,7 +3889,7 @@
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -3948,7 +3953,7 @@
         <v>68</v>
       </c>
       <c r="J28" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -4108,7 +4113,7 @@
         <v>8</v>
       </c>
       <c r="J33" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -4140,7 +4145,7 @@
         <v>54</v>
       </c>
       <c r="J34" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -4300,7 +4305,7 @@
         <v>8</v>
       </c>
       <c r="J39" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4408,7 +4413,7 @@
         <v>133</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>3</v>
@@ -4653,7 +4658,7 @@
         <v>8</v>
       </c>
       <c r="J51" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -4909,7 +4914,7 @@
         <v>8</v>
       </c>
       <c r="J59" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -4941,7 +4946,7 @@
         <v>40</v>
       </c>
       <c r="J60" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5069,7 +5074,7 @@
         <v>54</v>
       </c>
       <c r="J64" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5165,7 +5170,7 @@
         <v>8</v>
       </c>
       <c r="J67" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5293,7 +5298,7 @@
         <v>8</v>
       </c>
       <c r="J71" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5453,7 +5458,7 @@
         <v>54</v>
       </c>
       <c r="J76" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5517,7 +5522,7 @@
         <v>8</v>
       </c>
       <c r="J78" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5646,7 +5651,7 @@
         <v>24</v>
       </c>
       <c r="J83" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -5710,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="J85" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -10633,8 +10638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13432EB9-12D1-461D-8E87-0C40A7048F1D}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10665,7 +10670,7 @@
         <v>505</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>501</v>
@@ -11048,7 +11053,7 @@
         <v>635</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>612</v>
@@ -11170,19 +11175,19 @@
       <c r="K14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>648</v>
+      <c r="L14" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>649</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>650</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>2</v>
@@ -11194,10 +11199,10 @@
         <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>651</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>652</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>19</v>
@@ -11214,13 +11219,13 @@
     </row>
     <row r="16" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>416</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
@@ -11235,7 +11240,7 @@
         <v>376</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>242</v>
@@ -11252,13 +11257,13 @@
     </row>
     <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>657</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>658</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
@@ -11273,7 +11278,7 @@
         <v>301</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>248</v>
@@ -11290,13 +11295,13 @@
     </row>
     <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>662</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>
@@ -11311,7 +11316,7 @@
         <v>297</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>242</v>
@@ -11328,28 +11333,28 @@
     </row>
     <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>667</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>393</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>83</v>
@@ -11366,28 +11371,28 @@
     </row>
     <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>672</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>430</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>248</v>
@@ -11404,13 +11409,13 @@
     </row>
     <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>676</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>2</v>
@@ -11425,7 +11430,7 @@
         <v>391</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>242</v>
@@ -11442,13 +11447,13 @@
     </row>
     <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>680</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
@@ -11460,10 +11465,10 @@
         <v>134</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>682</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>50</v>
@@ -11480,13 +11485,13 @@
     </row>
     <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>685</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>2</v>
@@ -11501,7 +11506,7 @@
         <v>373</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>289</v>
@@ -11518,13 +11523,13 @@
     </row>
     <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>2</v>
@@ -11539,7 +11544,7 @@
         <v>349</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>248</v>
@@ -11556,13 +11561,13 @@
     </row>
     <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>692</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>2</v>
@@ -11574,10 +11579,10 @@
         <v>183</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>694</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>345</v>
@@ -11594,13 +11599,13 @@
     </row>
     <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>696</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>697</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>2</v>
@@ -11612,10 +11617,10 @@
         <v>122</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>699</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>12</v>
@@ -11632,13 +11637,13 @@
     </row>
     <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>702</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>2</v>
@@ -11653,7 +11658,7 @@
         <v>282</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>289</v>
@@ -11670,14 +11675,14 @@
     </row>
     <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>706</v>
-      </c>
       <c r="D28" s="1" t="s">
         <v>2</v>
       </c>
@@ -11685,13 +11690,13 @@
         <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>349</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>242</v>
@@ -11708,13 +11713,13 @@
     </row>
     <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>710</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>2</v>
@@ -11729,7 +11734,7 @@
         <v>430</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>47</v>
@@ -11746,13 +11751,13 @@
     </row>
     <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>713</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
@@ -11764,10 +11769,10 @@
         <v>205</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>715</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>242</v>
@@ -11784,13 +11789,13 @@
     </row>
     <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>718</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
@@ -11805,7 +11810,7 @@
         <v>349</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>12</v>
@@ -11822,13 +11827,13 @@
     </row>
     <row r="32" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>722</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>2</v>
@@ -11840,10 +11845,10 @@
         <v>28</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>724</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>248</v>
@@ -11860,13 +11865,13 @@
     </row>
     <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>727</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>2</v>
@@ -11881,7 +11886,7 @@
         <v>337</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>242</v>
@@ -11901,10 +11906,10 @@
         <v>45594</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>730</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>2</v>
@@ -11919,7 +11924,7 @@
         <v>458</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>242</v>
@@ -11936,13 +11941,13 @@
     </row>
     <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>733</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>734</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>2</v>
@@ -11957,7 +11962,7 @@
         <v>422</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>248</v>
@@ -11974,13 +11979,13 @@
     </row>
     <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>738</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>2</v>
@@ -11995,7 +12000,7 @@
         <v>285</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>242</v>
@@ -12012,28 +12017,28 @@
     </row>
     <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>601</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>742</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>743</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>50</v>
@@ -12050,13 +12055,13 @@
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>745</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>746</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>2</v>
@@ -12071,7 +12076,7 @@
         <v>430</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>248</v>
@@ -12088,13 +12093,13 @@
     </row>
     <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
@@ -12106,10 +12111,10 @@
         <v>336</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>751</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>12</v>
@@ -12118,7 +12123,7 @@
         <v>208</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>40</v>
@@ -12126,13 +12131,13 @@
     </row>
     <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>754</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>2</v>
@@ -12147,7 +12152,7 @@
         <v>346</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>47</v>
@@ -12156,7 +12161,7 @@
         <v>154</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>8</v>
@@ -12164,13 +12169,13 @@
     </row>
     <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>759</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>2</v>
@@ -12185,7 +12190,7 @@
         <v>301</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>50</v>
@@ -12194,7 +12199,7 @@
         <v>208</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>54</v>
@@ -12202,13 +12207,13 @@
     </row>
     <row r="42" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>763</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>2</v>
@@ -12223,7 +12228,7 @@
         <v>634</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>83</v>
@@ -12240,13 +12245,13 @@
     </row>
     <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>767</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>2</v>
@@ -12258,10 +12263,10 @@
         <v>60</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>769</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>303</v>
@@ -12278,13 +12283,13 @@
     </row>
     <row r="44" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>771</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>772</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>2</v>
@@ -12299,7 +12304,7 @@
         <v>282</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>74</v>
@@ -12308,7 +12313,7 @@
         <v>208</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>54</v>
@@ -12316,13 +12321,13 @@
     </row>
     <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>776</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>2</v>
@@ -12337,7 +12342,7 @@
         <v>349</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>248</v>
@@ -12354,13 +12359,13 @@
     </row>
     <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>2</v>
@@ -12375,7 +12380,7 @@
         <v>376</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>242</v>
@@ -12384,7 +12389,7 @@
         <v>208</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>244</v>
@@ -12428,7 +12433,7 @@
         <v>505</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>501</v>
@@ -12445,13 +12450,13 @@
     </row>
     <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>785</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -12466,7 +12471,7 @@
         <v>422</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>248</v>
@@ -12483,13 +12488,13 @@
     </row>
     <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>787</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>788</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -12501,10 +12506,10 @@
         <v>336</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>789</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>790</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>248</v>
@@ -12521,13 +12526,13 @@
     </row>
     <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>793</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -12542,10 +12547,10 @@
         <v>282</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>795</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>6</v>
@@ -12559,13 +12564,13 @@
     </row>
     <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>798</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -12580,7 +12585,7 @@
         <v>346</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>47</v>
@@ -12597,13 +12602,13 @@
     </row>
     <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>801</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>802</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
@@ -12618,7 +12623,7 @@
         <v>290</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>50</v>
@@ -12635,13 +12640,13 @@
     </row>
     <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>806</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
@@ -12656,7 +12661,7 @@
         <v>349</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>345</v>
@@ -12673,13 +12678,13 @@
     </row>
     <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>809</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>810</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
@@ -12694,7 +12699,7 @@
         <v>349</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>12</v>
@@ -12711,13 +12716,13 @@
     </row>
     <row r="9" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>813</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>814</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -12732,7 +12737,7 @@
         <v>297</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>242</v>
@@ -12749,13 +12754,13 @@
     </row>
     <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>817</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
@@ -12770,10 +12775,10 @@
         <v>373</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>818</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>819</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>208</v>
@@ -12787,13 +12792,13 @@
     </row>
     <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>821</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>822</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
@@ -12808,7 +12813,7 @@
         <v>349</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>242</v>
@@ -12840,24 +12845,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>840</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>842</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -12865,10 +12870,10 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -12876,10 +12881,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>845</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -12887,10 +12892,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -12898,10 +12903,10 @@
         <v>289</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -12909,10 +12914,10 @@
         <v>596</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>849</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -12920,10 +12925,10 @@
         <v>326</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -12931,10 +12936,10 @@
         <v>440</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -12942,10 +12947,10 @@
         <v>242</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -12953,10 +12958,10 @@
         <v>345</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -12964,10 +12969,10 @@
         <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -12975,21 +12980,21 @@
         <v>83</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -12997,21 +13002,21 @@
         <v>303</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -13019,10 +13024,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -13030,10 +13035,10 @@
         <v>248</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -13041,10 +13046,10 @@
         <v>74</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -13052,10 +13057,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -13063,10 +13068,10 @@
         <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -13074,10 +13079,10 @@
         <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>